<commit_message>
New translations name.xlsx (Portuguese, Brazilian)
</commit_message>
<xml_diff>
--- a/pt-BR/Traduzido/PTBR-Crowdin/Traduzido/PTBR/Lang/PTBR/Data/Name.xlsx
+++ b/pt-BR/Traduzido/PTBR-Crowdin/Traduzido/PTBR/Lang/PTBR/Data/Name.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isy\Documents\GitHub\elin-portugues-brasileiro\Original\Unificado\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Elin\Package\PTBR\Lang\PTBR\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E81D976-B2FD-456D-9E27-43026D52A31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6379EC3A-6193-449D-8469-87986BFFE386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17790" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10995" yWindow="1410" windowWidth="17790" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Name_EN" sheetId="1" r:id="rId1"/>
@@ -20,1590 +20,1596 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="530">
   <si>
     <t>a</t>
   </si>
   <si>
-    <t>ak</t>
-  </si>
-  <si>
-    <t>ay</t>
-  </si>
-  <si>
-    <t>as</t>
-  </si>
-  <si>
-    <t>azi</t>
-  </si>
-  <si>
-    <t>atta</t>
-  </si>
-  <si>
-    <t>adel</t>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Xe</t>
+  </si>
+  <si>
+    <t>ris</t>
+  </si>
+  <si>
+    <t>Ser</t>
+  </si>
+  <si>
+    <t>ion</t>
+  </si>
+  <si>
+    <t>Sk</t>
+  </si>
+  <si>
+    <t>cha</t>
+  </si>
+  <si>
+    <t>Da</t>
+  </si>
+  <si>
+    <t>ki</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>ke</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>yr</t>
+  </si>
+  <si>
+    <t>Fe</t>
+  </si>
+  <si>
+    <t>eo</t>
+  </si>
+  <si>
+    <t>Dae</t>
+  </si>
+  <si>
+    <t>las</t>
+  </si>
+  <si>
+    <t>Or</t>
+  </si>
+  <si>
+    <t>rys</t>
+  </si>
+  <si>
+    <t>Pho</t>
+  </si>
+  <si>
+    <t>io</t>
+  </si>
+  <si>
+    <t>Fen</t>
+  </si>
+  <si>
+    <t>rin</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>adi</t>
+  </si>
+  <si>
+    <t>Lir</t>
+  </si>
+  <si>
+    <t>la</t>
+  </si>
+  <si>
+    <t>Fr</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>aco</t>
+  </si>
+  <si>
+    <t>Dam</t>
+  </si>
+  <si>
+    <t>ya</t>
+  </si>
+  <si>
+    <t>Fa</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Ka</t>
+  </si>
+  <si>
+    <t>ke</t>
+  </si>
+  <si>
+    <t>Ty</t>
+  </si>
+  <si>
+    <t>ki</t>
+  </si>
+  <si>
+    <t>Th</t>
+  </si>
+  <si>
+    <t>iel</t>
+  </si>
+  <si>
+    <t>Ga</t>
+  </si>
+  <si>
+    <t>uto</t>
+  </si>
+  <si>
+    <t>Ka</t>
+  </si>
+  <si>
+    <t>adi</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>lix</t>
+  </si>
+  <si>
+    <t>Ar</t>
+  </si>
+  <si>
+    <t>eo</t>
+  </si>
+  <si>
+    <t>Tho</t>
+  </si>
+  <si>
+    <t>uka</t>
+  </si>
+  <si>
+    <t>El</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>Le</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Gw</t>
+  </si>
+  <si>
+    <t>ron</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Rag</t>
+  </si>
+  <si>
+    <t>aus</t>
+  </si>
+  <si>
+    <t>Sk</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>ena</t>
+  </si>
+  <si>
+    <t>Za</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Tob</t>
+  </si>
+  <si>
+    <t>zo</t>
+  </si>
+  <si>
+    <t>So</t>
+  </si>
+  <si>
+    <t>nte</t>
+  </si>
+  <si>
+    <t>Sor</t>
+  </si>
+  <si>
+    <t>adi</t>
+  </si>
+  <si>
+    <t>Ta</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Xe</t>
+  </si>
+  <si>
+    <t>ene</t>
+  </si>
+  <si>
+    <t>Mi</t>
+  </si>
+  <si>
+    <t>lia</t>
+  </si>
+  <si>
+    <t>Ay</t>
+  </si>
+  <si>
+    <t>io</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>ris</t>
+  </si>
+  <si>
+    <t>Nar</t>
+  </si>
+  <si>
+    <t>ene</t>
+  </si>
+  <si>
+    <t>Ae</t>
+  </si>
+  <si>
+    <t>ven</t>
+  </si>
+  <si>
+    <t>Fen</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Ezr</t>
+  </si>
+  <si>
+    <t>cha</t>
+  </si>
+  <si>
+    <t>Al</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Th</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Kl</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>Or</t>
+  </si>
+  <si>
+    <t>ebe</t>
+  </si>
+  <si>
+    <t>Ni</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Dae</t>
+  </si>
+  <si>
+    <t>ien</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>éo</t>
+  </si>
+  <si>
+    <t>Sk</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Cl</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Sor</t>
+  </si>
+  <si>
+    <t>aco</t>
+  </si>
+  <si>
+    <t>Br</t>
+  </si>
+  <si>
+    <t>io</t>
+  </si>
+  <si>
+    <t>Ga</t>
+  </si>
+  <si>
+    <t>aus</t>
+  </si>
+  <si>
+    <t>Dam</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>Br</t>
+  </si>
+  <si>
+    <t>cha</t>
+  </si>
+  <si>
+    <t>Zi</t>
+  </si>
+  <si>
+    <t>eya</t>
+  </si>
+  <si>
+    <t>Ax</t>
+  </si>
+  <si>
+    <t>th</t>
+  </si>
+  <si>
+    <t>Ri</t>
+  </si>
+  <si>
+    <t>iel</t>
+  </si>
+  <si>
+    <t>Sel</t>
+  </si>
+  <si>
+    <t>lia</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>éo</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Ta</t>
+  </si>
+  <si>
+    <t>la</t>
+  </si>
+  <si>
+    <t>Da</t>
+  </si>
+  <si>
+    <t>este</t>
+  </si>
+  <si>
+    <t>As</t>
+  </si>
+  <si>
+    <t>ya</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>Ro</t>
+  </si>
+  <si>
+    <t>ona</t>
+  </si>
+  <si>
+    <t>Tho</t>
+  </si>
+  <si>
+    <t>ena</t>
+  </si>
+  <si>
+    <t>Cas</t>
+  </si>
+  <si>
+    <t>sian</t>
+  </si>
+  <si>
+    <t>Od</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>El</t>
+  </si>
+  <si>
+    <t>ri</t>
+  </si>
+  <si>
+    <t>Cas</t>
+  </si>
+  <si>
+    <t>lo</t>
+  </si>
+  <si>
+    <t>Ez</t>
+  </si>
+  <si>
+    <t>ye</t>
+  </si>
+  <si>
+    <t>Lu</t>
+  </si>
+  <si>
+    <t>la</t>
+  </si>
+  <si>
+    <t>En</t>
+  </si>
+  <si>
+    <t>ei</t>
+  </si>
+  <si>
+    <t>Ga</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Fe</t>
+  </si>
+  <si>
+    <t>yr</t>
+  </si>
+  <si>
+    <t>Xe</t>
+  </si>
+  <si>
+    <t>iel</t>
+  </si>
+  <si>
+    <t>Se</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>eya</t>
+  </si>
+  <si>
+    <t>Za</t>
+  </si>
+  <si>
+    <t>ien</t>
+  </si>
+  <si>
+    <t>Ath</t>
+  </si>
+  <si>
+    <t>yx</t>
+  </si>
+  <si>
+    <t>Sel</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>Ro</t>
+  </si>
+  <si>
+    <t>leb</t>
+  </si>
+  <si>
+    <t>Or</t>
+  </si>
+  <si>
+    <t>uto</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>th</t>
+  </si>
+  <si>
+    <t>El</t>
+  </si>
+  <si>
+    <t>ian</t>
+  </si>
+  <si>
+    <t>Yu</t>
+  </si>
+  <si>
+    <t>omi</t>
+  </si>
+  <si>
+    <t>Ezr</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>Ze</t>
+  </si>
+  <si>
+    <t>ena</t>
+  </si>
+  <si>
+    <t>Xe</t>
+  </si>
+  <si>
+    <t>sian</t>
+  </si>
+  <si>
+    <t>Se</t>
+  </si>
+  <si>
+    <t>nte</t>
+  </si>
+  <si>
+    <t>Ze</t>
+  </si>
+  <si>
+    <t>ion</t>
+  </si>
+  <si>
+    <t>Jas</t>
+  </si>
+  <si>
+    <t>lia</t>
+  </si>
+  <si>
+    <t>Ty</t>
+  </si>
+  <si>
+    <t>rin</t>
+  </si>
+  <si>
+    <t>Am</t>
+  </si>
+  <si>
+    <t>ona</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>ena</t>
+  </si>
+  <si>
+    <t>Ala</t>
+  </si>
+  <si>
+    <t>yla</t>
+  </si>
+  <si>
+    <t>Luc</t>
   </si>
   <si>
     <t>an</t>
   </si>
   <si>
-    <t>ane</t>
-  </si>
-  <si>
-    <t>ig</t>
-  </si>
-  <si>
-    <t>aba</t>
-  </si>
-  <si>
-    <t>inne</t>
-  </si>
-  <si>
-    <t>af</t>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>ya</t>
+  </si>
+  <si>
+    <t>Cas</t>
+  </si>
+  <si>
+    <t>an</t>
+  </si>
+  <si>
+    <t>Da</t>
   </si>
   <si>
     <t>in</t>
   </si>
   <si>
-    <t>ahe</t>
-  </si>
-  <si>
-    <t>ug</t>
-  </si>
-  <si>
-    <t>ama</t>
-  </si>
-  <si>
-    <t>un</t>
+    <t>Dr</t>
+  </si>
+  <si>
+    <t>uto</t>
+  </si>
+  <si>
+    <t>Tha</t>
+  </si>
+  <si>
+    <t>ric</t>
+  </si>
+  <si>
+    <t>Ae</t>
+  </si>
+  <si>
+    <t>th</t>
+  </si>
+  <si>
+    <t>Ni</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Ei</t>
+  </si>
+  <si>
+    <t>iel</t>
+  </si>
+  <si>
+    <t>Gw</t>
+  </si>
+  <si>
+    <t>eo</t>
+  </si>
+  <si>
+    <t>Dr</t>
+  </si>
+  <si>
+    <t>ya</t>
+  </si>
+  <si>
+    <t>Cel</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Lu</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>Zi</t>
+  </si>
+  <si>
+    <t>sia</t>
+  </si>
+  <si>
+    <t>Ez</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Tho</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Se</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Ga</t>
+  </si>
+  <si>
+    <t>ena</t>
+  </si>
+  <si>
+    <t>Za</t>
+  </si>
+  <si>
+    <t>ai</t>
+  </si>
+  <si>
+    <t>So</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>Sak</t>
+  </si>
+  <si>
+    <t>nar</t>
+  </si>
+  <si>
+    <t>Ra</t>
+  </si>
+  <si>
+    <t>ven</t>
+  </si>
+  <si>
+    <t>As</t>
+  </si>
+  <si>
+    <t>ai</t>
+  </si>
+  <si>
+    <t>Ni</t>
+  </si>
+  <si>
+    <t>ira</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Cas</t>
+  </si>
+  <si>
+    <t>ion</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>zo</t>
+  </si>
+  <si>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>ri</t>
+  </si>
+  <si>
+    <t>Al</t>
+  </si>
+  <si>
+    <t>la</t>
+  </si>
+  <si>
+    <t>Yu</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Ri</t>
+  </si>
+  <si>
+    <t>ron</t>
+  </si>
+  <si>
+    <t>Rag</t>
+  </si>
+  <si>
+    <t>ias</t>
+  </si>
+  <si>
+    <t>Lir</t>
+  </si>
+  <si>
+    <t>ien</t>
+  </si>
+  <si>
+    <t>Ri</t>
+  </si>
+  <si>
+    <t>ian</t>
+  </si>
+  <si>
+    <t>Ser</t>
+  </si>
+  <si>
+    <t>ia</t>
+  </si>
+  <si>
+    <t>Luc</t>
+  </si>
+  <si>
+    <t>eo</t>
+  </si>
+  <si>
+    <t>Kl</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>Luc</t>
+  </si>
+  <si>
+    <t>lia</t>
+  </si>
+  <si>
+    <t>Cae</t>
+  </si>
+  <si>
+    <t>ias</t>
+  </si>
+  <si>
+    <t>Ra</t>
+  </si>
+  <si>
+    <t>adi</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
   <si>
     <t>ara</t>
   </si>
   <si>
-    <t>es</t>
-  </si>
-  <si>
-    <t>ali</t>
-  </si>
-  <si>
-    <t>eth</t>
-  </si>
-  <si>
-    <t>al</t>
-  </si>
-  <si>
-    <t>etta</t>
-  </si>
-  <si>
-    <t>are</t>
+    <t>Nar</t>
+  </si>
+  <si>
+    <t>lix</t>
+  </si>
+  <si>
+    <t>Ei</t>
+  </si>
+  <si>
+    <t>ena</t>
+  </si>
+  <si>
+    <t>Lu</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>Ez</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Ty</t>
+  </si>
+  <si>
+    <t>eo</t>
+  </si>
+  <si>
+    <t>Ak</t>
+  </si>
+  <si>
+    <t>va</t>
+  </si>
+  <si>
+    <t>Ni</t>
+  </si>
+  <si>
+    <t>ina</t>
+  </si>
+  <si>
+    <t>Le</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Le</t>
+  </si>
+  <si>
+    <t>eve</t>
+  </si>
+  <si>
+    <t>Ga</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>Cas</t>
+  </si>
+  <si>
+    <t>eo</t>
+  </si>
+  <si>
+    <t>Mi</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Ve</t>
+  </si>
+  <si>
+    <t>iel</t>
+  </si>
+  <si>
+    <t>Se</t>
+  </si>
+  <si>
+    <t>aco</t>
+  </si>
+  <si>
+    <t>Ezr</t>
+  </si>
+  <si>
+    <t>ien</t>
+  </si>
+  <si>
+    <t>Ra</t>
+  </si>
+  <si>
+    <t>ira</t>
+  </si>
+  <si>
+    <t>Se</t>
+  </si>
+  <si>
+    <t>ris</t>
+  </si>
+  <si>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>ah</t>
+  </si>
+  <si>
+    <t>Cl</t>
+  </si>
+  <si>
+    <t>ion</t>
+  </si>
+  <si>
+    <t>Or</t>
+  </si>
+  <si>
+    <t>ya</t>
+  </si>
+  <si>
+    <t>Ay</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>Sor</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>El</t>
+  </si>
+  <si>
+    <t>leb</t>
+  </si>
+  <si>
+    <t>En</t>
+  </si>
+  <si>
+    <t>ena</t>
+  </si>
+  <si>
+    <t>Ka</t>
+  </si>
+  <si>
+    <t>va</t>
+  </si>
+  <si>
+    <t>Ki</t>
+  </si>
+  <si>
+    <t>ura</t>
+  </si>
+  <si>
+    <t>Ty</t>
+  </si>
+  <si>
+    <t>wan</t>
+  </si>
+  <si>
+    <t>Ar</t>
+  </si>
+  <si>
+    <t>ura</t>
+  </si>
+  <si>
+    <t>Ro</t>
+  </si>
+  <si>
+    <t>ven</t>
+  </si>
+  <si>
+    <t>Ax</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Ta</t>
+  </si>
+  <si>
+    <t>la</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Nar</t>
+  </si>
+  <si>
+    <t>lo</t>
+  </si>
+  <si>
+    <t>Sor</t>
+  </si>
+  <si>
+    <t>yla</t>
+  </si>
+  <si>
+    <t>Yu</t>
+  </si>
+  <si>
+    <t>ris</t>
+  </si>
+  <si>
+    <t>Ei</t>
+  </si>
+  <si>
+    <t>lia</t>
+  </si>
+  <si>
+    <t>Ezr</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Ez</t>
+  </si>
+  <si>
+    <t>wan</t>
+  </si>
+  <si>
+    <t>El</t>
+  </si>
+  <si>
+    <t>vi</t>
+  </si>
+  <si>
+    <t>Lo</t>
+  </si>
+  <si>
+    <t>ebe</t>
+  </si>
+  <si>
+    <t>Fen</t>
+  </si>
+  <si>
+    <t>ona</t>
+  </si>
+  <si>
+    <t>Od</t>
+  </si>
+  <si>
+    <t>th</t>
+  </si>
+  <si>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>eya</t>
+  </si>
+  <si>
+    <t>Ez</t>
+  </si>
+  <si>
+    <t>yn</t>
+  </si>
+  <si>
+    <t>Luc</t>
+  </si>
+  <si>
+    <t>rys</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>ion</t>
+  </si>
+  <si>
+    <t>Za</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>Ay</t>
+  </si>
+  <si>
+    <t>iel</t>
+  </si>
+  <si>
+    <t>Ser</t>
+  </si>
+  <si>
+    <t>th</t>
+  </si>
+  <si>
+    <t>Ax</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>Or</t>
+  </si>
+  <si>
+    <t>lum</t>
+  </si>
+  <si>
+    <t>Kl</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>Cl</t>
   </si>
   <si>
     <t>en</t>
   </si>
   <si>
-    <t>alec</t>
-  </si>
-  <si>
-    <t>ord</t>
-  </si>
-  <si>
-    <t>arro</t>
-  </si>
-  <si>
-    <t>os</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>oz</t>
-  </si>
-  <si>
-    <t>io</t>
-  </si>
-  <si>
-    <t>otta</t>
-  </si>
-  <si>
-    <t>ish</t>
+    <t>Dae</t>
+  </si>
+  <si>
+    <t>ia</t>
+  </si>
+  <si>
+    <t>Or</t>
+  </si>
+  <si>
+    <t>uto</t>
+  </si>
+  <si>
+    <t>Ka</t>
+  </si>
+  <si>
+    <t>leb</t>
+  </si>
+  <si>
+    <t>Ei</t>
+  </si>
+  <si>
+    <t>lix</t>
+  </si>
+  <si>
+    <t>Ri</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Th</t>
+  </si>
+  <si>
+    <t>ias</t>
+  </si>
+  <si>
+    <t>Ir</t>
+  </si>
+  <si>
+    <t>uka</t>
+  </si>
+  <si>
+    <t>Ak</t>
+  </si>
+  <si>
+    <t>ah</t>
+  </si>
+  <si>
+    <t>Ay</t>
+  </si>
+  <si>
+    <t>ian</t>
+  </si>
+  <si>
+    <t>Fr</t>
+  </si>
+  <si>
+    <t>ai</t>
+  </si>
+  <si>
+    <t>Mi</t>
+  </si>
+  <si>
+    <t>ki</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>ke</t>
+  </si>
+  <si>
+    <t>Mi</t>
+  </si>
+  <si>
+    <t>ric</t>
+  </si>
+  <si>
+    <t>Ly</t>
+  </si>
+  <si>
+    <t>ian</t>
+  </si>
+  <si>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>lix</t>
+  </si>
+  <si>
+    <t>Ser</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>éo</t>
+  </si>
+  <si>
+    <t>Ak</t>
+  </si>
+  <si>
+    <t>ia</t>
+  </si>
+  <si>
+    <t>Sy</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Ka</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>ina</t>
+  </si>
+  <si>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>yn</t>
+  </si>
+  <si>
+    <t>Ser</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>Za</t>
+  </si>
+  <si>
+    <t>nte</t>
+  </si>
+  <si>
+    <t>Le</t>
+  </si>
+  <si>
+    <t>th</t>
+  </si>
+  <si>
+    <t>Od</t>
+  </si>
+  <si>
+    <t>ena</t>
+  </si>
+  <si>
+    <t>Sk</t>
+  </si>
+  <si>
+    <t>ena</t>
+  </si>
+  <si>
+    <t>Ze</t>
+  </si>
+  <si>
+    <t>ia</t>
+  </si>
+  <si>
+    <t>Fe</t>
+  </si>
+  <si>
+    <t>nar</t>
+  </si>
+  <si>
+    <t>Fen</t>
+  </si>
+  <si>
+    <t>nte</t>
+  </si>
+  <si>
+    <t>Se</t>
+  </si>
+  <si>
+    <t>lia</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>ia</t>
+  </si>
+  <si>
+    <t>Da</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Ve</t>
+  </si>
+  <si>
+    <t>ebe</t>
+  </si>
+  <si>
+    <t>Ga</t>
+  </si>
+  <si>
+    <t>per</t>
+  </si>
+  <si>
+    <t>Lir</t>
+  </si>
+  <si>
+    <t>ven</t>
+  </si>
+  <si>
+    <t>El</t>
+  </si>
+  <si>
+    <t>aus</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
   <si>
     <t>on</t>
   </si>
   <si>
-    <t>if</t>
-  </si>
-  <si>
-    <t>ga</t>
-  </si>
-  <si>
-    <t>iv</t>
-  </si>
-  <si>
-    <t>gar</t>
-  </si>
-  <si>
-    <t>il</t>
-  </si>
-  <si>
-    <t>gas</t>
-  </si>
-  <si>
-    <t>ir</t>
-  </si>
-  <si>
-    <t>cas</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>gan</t>
-  </si>
-  <si>
-    <t>ub</t>
-  </si>
-  <si>
-    <t>gy</t>
-  </si>
-  <si>
-    <t>ur</t>
-  </si>
-  <si>
-    <t>gis</t>
-  </si>
-  <si>
-    <t>ula</t>
-  </si>
-  <si>
-    <t>gistan</t>
-  </si>
-  <si>
-    <t>uli</t>
-  </si>
-  <si>
-    <t>gin</t>
-  </si>
-  <si>
-    <t>ul</t>
-  </si>
-  <si>
-    <t>keyro</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>gues</t>
-  </si>
-  <si>
-    <t>ey</t>
-  </si>
-  <si>
-    <t>guen</t>
-  </si>
-  <si>
-    <t>eym</t>
-  </si>
-  <si>
-    <t>co</t>
-  </si>
-  <si>
-    <t>edo</t>
-  </si>
-  <si>
-    <t>cord</t>
-  </si>
-  <si>
-    <t>eva</t>
-  </si>
-  <si>
-    <t>goth</t>
-  </si>
-  <si>
-    <t>evo</t>
-  </si>
-  <si>
-    <t>cold</t>
-  </si>
-  <si>
-    <t>era</t>
-  </si>
-  <si>
-    <t>cory</t>
-  </si>
-  <si>
-    <t>eli</t>
-  </si>
-  <si>
-    <t>cole</t>
-  </si>
-  <si>
-    <t>elis</t>
-  </si>
-  <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>ero</t>
-  </si>
-  <si>
-    <t>za</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t>sar</t>
-  </si>
-  <si>
-    <t>oy</t>
-  </si>
-  <si>
-    <t>zard</t>
-  </si>
-  <si>
-    <t>og</t>
-  </si>
-  <si>
-    <t>sard</t>
-  </si>
-  <si>
-    <t>os</t>
-  </si>
-  <si>
-    <t>zas</t>
-  </si>
-  <si>
-    <t>oz</t>
-  </si>
-  <si>
-    <t>sammy</t>
-  </si>
-  <si>
-    <t>ozo</t>
-  </si>
-  <si>
-    <t>zastan</t>
-  </si>
-  <si>
-    <t>ody</t>
-  </si>
-  <si>
-    <t>thandla</t>
-  </si>
-  <si>
-    <t>obe</t>
-  </si>
-  <si>
-    <t>sand</t>
-  </si>
-  <si>
-    <t>omi</t>
-  </si>
-  <si>
-    <t>seek</t>
-  </si>
-  <si>
-    <t>ol</t>
-  </si>
-  <si>
-    <t>sierra</t>
-  </si>
-  <si>
-    <t>ka</t>
-  </si>
-  <si>
-    <t>siel</t>
-  </si>
-  <si>
-    <t>ga</t>
-  </si>
-  <si>
-    <t>ziss</t>
-  </si>
-  <si>
-    <t>kay</t>
-  </si>
-  <si>
-    <t>sid</t>
-  </si>
-  <si>
-    <t>casa</t>
-  </si>
-  <si>
-    <t>sha</t>
-  </si>
-  <si>
-    <t>cas</t>
-  </si>
-  <si>
-    <t>shark</t>
-  </si>
-  <si>
-    <t>kas</t>
-  </si>
-  <si>
-    <t>siss</t>
-  </si>
-  <si>
-    <t>kaz</t>
-  </si>
-  <si>
-    <t>shack</t>
-  </si>
-  <si>
-    <t>kab</t>
-  </si>
-  <si>
-    <t>shy</t>
-  </si>
-  <si>
-    <t>caf</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>cav</t>
-  </si>
-  <si>
-    <t>suk</t>
-  </si>
-  <si>
-    <t>kanz</t>
-  </si>
-  <si>
-    <t>zess</t>
-  </si>
-  <si>
-    <t>ganda</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>ky</t>
-  </si>
-  <si>
-    <t>cess</t>
-  </si>
-  <si>
-    <t>gy</t>
-  </si>
-  <si>
-    <t>sor</t>
-  </si>
-  <si>
-    <t>gik</t>
-  </si>
-  <si>
-    <t>sorc</t>
-  </si>
-  <si>
-    <t>kiz</t>
-  </si>
-  <si>
-    <t>sord</t>
-  </si>
-  <si>
-    <t>giz</t>
-  </si>
-  <si>
-    <t>zof</t>
-  </si>
-  <si>
-    <t>kis</t>
-  </si>
-  <si>
-    <t>sony</t>
-  </si>
-  <si>
-    <t>gis</t>
-  </si>
-  <si>
-    <t>ta</t>
-  </si>
-  <si>
-    <t>cu</t>
-  </si>
-  <si>
-    <t>dar</t>
-  </si>
-  <si>
-    <t>gu</t>
-  </si>
-  <si>
-    <t>tan</t>
-  </si>
-  <si>
-    <t>kut</t>
-  </si>
-  <si>
-    <t>daos</t>
-  </si>
-  <si>
-    <t>kuf</t>
-  </si>
-  <si>
-    <t>daora</t>
-  </si>
-  <si>
-    <t>ke</t>
-  </si>
-  <si>
-    <t>deth</t>
-  </si>
-  <si>
-    <t>ge</t>
-  </si>
-  <si>
-    <t>dath</t>
-  </si>
-  <si>
-    <t>kef</t>
-  </si>
-  <si>
-    <t>tam</t>
-  </si>
-  <si>
-    <t>kor</t>
-  </si>
-  <si>
-    <t>tali</t>
-  </si>
-  <si>
-    <t>cor</t>
-  </si>
-  <si>
-    <t>dark</t>
-  </si>
-  <si>
-    <t>go</t>
-  </si>
-  <si>
-    <t>dan</t>
-  </si>
-  <si>
-    <t>kof</t>
-  </si>
-  <si>
-    <t>tis</t>
-  </si>
-  <si>
-    <t>kov</t>
-  </si>
-  <si>
-    <t>tin</t>
-  </si>
-  <si>
-    <t>kor</t>
-  </si>
-  <si>
-    <t>kka</t>
-  </si>
-  <si>
-    <t>gor</t>
-  </si>
-  <si>
-    <t>decker</t>
-  </si>
-  <si>
-    <t>gorra</t>
-  </si>
-  <si>
-    <t>cker</t>
-  </si>
-  <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>tuen</t>
-  </si>
-  <si>
-    <t>za</t>
-  </si>
-  <si>
-    <t>kor</t>
-  </si>
-  <si>
-    <t>say</t>
-  </si>
-  <si>
-    <t>tta</t>
-  </si>
-  <si>
-    <t>sazi</t>
-  </si>
-  <si>
-    <t>ty</t>
-  </si>
-  <si>
-    <t>sama</t>
-  </si>
-  <si>
-    <t>tty</t>
-  </si>
-  <si>
-    <t>samo</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>sar</t>
-  </si>
-  <si>
-    <t>tto</t>
-  </si>
-  <si>
-    <t>si</t>
-  </si>
-  <si>
-    <t>den</t>
-  </si>
-  <si>
-    <t>zi</t>
-  </si>
-  <si>
-    <t>dear</t>
-  </si>
-  <si>
-    <t>sha</t>
-  </si>
-  <si>
-    <t>dey</t>
-  </si>
-  <si>
-    <t>shu</t>
-  </si>
-  <si>
-    <t>cis</t>
-  </si>
-  <si>
-    <t>sho</t>
-  </si>
-  <si>
-    <t>dis</t>
-  </si>
-  <si>
-    <t>jil</t>
-  </si>
-  <si>
-    <t>din</t>
-  </si>
-  <si>
-    <t>su</t>
-  </si>
-  <si>
-    <t>deos</t>
-  </si>
-  <si>
-    <t>zu</t>
-  </si>
-  <si>
-    <t>destan</t>
-  </si>
-  <si>
-    <t>se</t>
-  </si>
-  <si>
-    <t>delia</t>
-  </si>
-  <si>
-    <t>ze</t>
-  </si>
-  <si>
-    <t>ten</t>
-  </si>
-  <si>
-    <t>sey</t>
-  </si>
-  <si>
-    <t>tor</t>
-  </si>
-  <si>
-    <t>say</t>
-  </si>
-  <si>
-    <t>dor</t>
-  </si>
-  <si>
-    <t>sesa</t>
-  </si>
-  <si>
-    <t>dorre</t>
-  </si>
-  <si>
-    <t>ces</t>
-  </si>
-  <si>
-    <t>toli</t>
-  </si>
-  <si>
-    <t>sez</t>
-  </si>
-  <si>
-    <t>don</t>
-  </si>
-  <si>
-    <t>sem</t>
-  </si>
-  <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>ser</t>
-  </si>
-  <si>
-    <t>nart</t>
-  </si>
-  <si>
-    <t>cero</t>
-  </si>
-  <si>
-    <t>nert</t>
-  </si>
-  <si>
-    <t>so</t>
-  </si>
-  <si>
-    <t>nerd</t>
-  </si>
-  <si>
-    <t>sor</t>
-  </si>
-  <si>
-    <t>nail</t>
-  </si>
-  <si>
-    <t>soy</t>
-  </si>
-  <si>
-    <t>nas</t>
-  </si>
-  <si>
-    <t>da</t>
-  </si>
-  <si>
-    <t>nakk</t>
-  </si>
-  <si>
-    <t>ti</t>
-  </si>
-  <si>
-    <t>naf</t>
-  </si>
-  <si>
-    <t>tar</t>
-  </si>
-  <si>
-    <t>narc</t>
-  </si>
-  <si>
-    <t>tam</t>
-  </si>
-  <si>
-    <t>nald</t>
-  </si>
-  <si>
-    <t>die</t>
-  </si>
-  <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>tao</t>
-  </si>
-  <si>
-    <t>ny</t>
-  </si>
-  <si>
-    <t>dar</t>
-  </si>
-  <si>
-    <t>nick</t>
-  </si>
-  <si>
-    <t>chi</t>
-  </si>
-  <si>
-    <t>ne</t>
-  </si>
-  <si>
-    <t>cha</t>
-  </si>
-  <si>
-    <t>nail</t>
-  </si>
-  <si>
-    <t>chur</t>
-  </si>
-  <si>
-    <t>ned</t>
-  </si>
-  <si>
-    <t>chor</t>
-  </si>
-  <si>
-    <t>neck</t>
-  </si>
-  <si>
-    <t>tur</t>
-  </si>
-  <si>
-    <t>nes</t>
-  </si>
-  <si>
-    <t>dur</t>
-  </si>
-  <si>
-    <t>nack</t>
-  </si>
-  <si>
-    <t>te</t>
-  </si>
-  <si>
-    <t>nel</t>
-  </si>
-  <si>
-    <t>dey</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>del</t>
-  </si>
-  <si>
-    <t>noir</t>
-  </si>
-  <si>
-    <t>teo</t>
-  </si>
-  <si>
-    <t>nor</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>nert</t>
-  </si>
-  <si>
-    <t>do</t>
-  </si>
-  <si>
-    <t>nort</t>
-  </si>
-  <si>
-    <t>tod</t>
-  </si>
-  <si>
-    <t>nord</t>
-  </si>
-  <si>
-    <t>tomy</t>
-  </si>
-  <si>
-    <t>nock</t>
-  </si>
-  <si>
-    <t>tom</t>
-  </si>
-  <si>
-    <t>nof</t>
-  </si>
-  <si>
-    <t>tol</t>
-  </si>
-  <si>
-    <t>nold</t>
-  </si>
-  <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>non</t>
-  </si>
-  <si>
-    <t>nag</t>
-  </si>
-  <si>
-    <t>by</t>
-  </si>
-  <si>
-    <t>nas</t>
-  </si>
-  <si>
-    <t>berg</t>
-  </si>
-  <si>
-    <t>naz</t>
-  </si>
-  <si>
-    <t>hert</t>
-  </si>
-  <si>
-    <t>nab</t>
-  </si>
-  <si>
-    <t>hart</t>
-  </si>
-  <si>
-    <t>nar</t>
-  </si>
-  <si>
-    <t>bird</t>
-  </si>
-  <si>
-    <t>ni</t>
-  </si>
-  <si>
-    <t>hard</t>
-  </si>
-  <si>
-    <t>nico</t>
-  </si>
-  <si>
-    <t>hael</t>
-  </si>
-  <si>
-    <t>nis</t>
-  </si>
-  <si>
-    <t>heal</t>
-  </si>
-  <si>
-    <t>nu</t>
-  </si>
-  <si>
-    <t>hack</t>
-  </si>
-  <si>
-    <t>ne</t>
-  </si>
-  <si>
-    <t>had</t>
-  </si>
-  <si>
-    <t>nel</t>
-  </si>
-  <si>
-    <t>vamos</t>
-  </si>
-  <si>
-    <t>nebi</t>
-  </si>
-  <si>
-    <t>halt</t>
-  </si>
-  <si>
-    <t>nero</t>
-  </si>
-  <si>
-    <t>bald</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>ban</t>
-  </si>
-  <si>
-    <t>nor</t>
-  </si>
-  <si>
-    <t>pan</t>
-  </si>
-  <si>
-    <t>ha</t>
-  </si>
-  <si>
-    <t>han</t>
-  </si>
-  <si>
-    <t>ba</t>
-  </si>
-  <si>
-    <t>via</t>
-  </si>
-  <si>
-    <t>pa</t>
-  </si>
-  <si>
-    <t>vy</t>
-  </si>
-  <si>
-    <t>hay</t>
-  </si>
-  <si>
-    <t>vis</t>
-  </si>
-  <si>
-    <t>hi</t>
-  </si>
-  <si>
-    <t>bit</t>
-  </si>
-  <si>
-    <t>bi</t>
-  </si>
-  <si>
-    <t>hymos</t>
-  </si>
-  <si>
-    <t>pi</t>
-  </si>
-  <si>
-    <t>pin</t>
-  </si>
-  <si>
-    <t>fu</t>
-  </si>
-  <si>
-    <t>vin</t>
-  </si>
-  <si>
-    <t>vu</t>
-  </si>
-  <si>
-    <t>far</t>
-  </si>
-  <si>
-    <t>pu</t>
-  </si>
-  <si>
-    <t>fael</t>
-  </si>
-  <si>
-    <t>fa</t>
-  </si>
-  <si>
-    <t>fous</t>
-  </si>
-  <si>
-    <t>fy</t>
-  </si>
-  <si>
-    <t>fas</t>
-  </si>
-  <si>
-    <t>fey</t>
-  </si>
-  <si>
-    <t>fy</t>
-  </si>
-  <si>
-    <t>for</t>
-  </si>
-  <si>
-    <t>fis</t>
-  </si>
-  <si>
-    <t>fleo</t>
-  </si>
-  <si>
-    <t>fuga</t>
-  </si>
-  <si>
-    <t>flea</t>
-  </si>
-  <si>
-    <t>fess</t>
-  </si>
-  <si>
-    <t>frey</t>
-  </si>
-  <si>
-    <t>for</t>
-  </si>
-  <si>
-    <t>frea</t>
-  </si>
-  <si>
-    <t>fon</t>
-  </si>
-  <si>
-    <t>he</t>
-  </si>
-  <si>
-    <t>forse</t>
-  </si>
-  <si>
-    <t>hes</t>
-  </si>
-  <si>
-    <t>ford</t>
-  </si>
-  <si>
-    <t>pe</t>
-  </si>
-  <si>
-    <t>feus</t>
-  </si>
-  <si>
-    <t>hel</t>
-  </si>
-  <si>
-    <t>hock</t>
-  </si>
-  <si>
-    <t>bel</t>
-  </si>
-  <si>
-    <t>bear</t>
-  </si>
-  <si>
-    <t>ho</t>
-  </si>
-  <si>
-    <t>beth</t>
-  </si>
-  <si>
-    <t>vo</t>
-  </si>
-  <si>
-    <t>beck</t>
-  </si>
-  <si>
-    <t>po</t>
-  </si>
-  <si>
-    <t>bed</t>
-  </si>
-  <si>
-    <t>ma</t>
-  </si>
-  <si>
-    <t>hed</t>
-  </si>
-  <si>
-    <t>mi</t>
-  </si>
-  <si>
-    <t>berk</t>
-  </si>
-  <si>
-    <t>mis</t>
-  </si>
-  <si>
-    <t>belt</t>
-  </si>
-  <si>
-    <t>mish</t>
-  </si>
-  <si>
-    <t>bor</t>
-  </si>
-  <si>
-    <t>misha</t>
-  </si>
-  <si>
-    <t>hawk</t>
-  </si>
-  <si>
-    <t>mys</t>
-  </si>
-  <si>
-    <t>horse</t>
-  </si>
-  <si>
-    <t>mu</t>
-  </si>
-  <si>
-    <t>boss</t>
-  </si>
-  <si>
-    <t>me</t>
-  </si>
-  <si>
-    <t>bon</t>
-  </si>
-  <si>
-    <t>mo</t>
-  </si>
-  <si>
-    <t>pond</t>
-  </si>
-  <si>
-    <t>mona</t>
-  </si>
-  <si>
-    <t>my</t>
-  </si>
-  <si>
-    <t>ya</t>
-  </si>
-  <si>
-    <t>miss</t>
-  </si>
-  <si>
-    <t>ju</t>
-  </si>
-  <si>
-    <t>mia</t>
-  </si>
-  <si>
-    <t>jo</t>
-  </si>
-  <si>
-    <t>mick</t>
+    <t>Ir</t>
+  </si>
+  <si>
+    <t>ei</t>
+  </si>
+  <si>
+    <t>Tha</t>
   </si>
   <si>
     <t>ra</t>
   </si>
   <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>rai</t>
-  </si>
-  <si>
-    <t>mer</t>
-  </si>
-  <si>
-    <t>reia</t>
-  </si>
-  <si>
-    <t>mos</t>
-  </si>
-  <si>
-    <t>lio</t>
-  </si>
-  <si>
-    <t>mes</t>
-  </si>
-  <si>
-    <t>laz</t>
-  </si>
-  <si>
-    <t>mock</t>
-  </si>
-  <si>
-    <t>li</t>
-  </si>
-  <si>
-    <t>mof</t>
-  </si>
-  <si>
-    <t>lu</t>
-  </si>
-  <si>
-    <t>ya</t>
-  </si>
-  <si>
-    <t>le</t>
-  </si>
-  <si>
-    <t>yas</t>
-  </si>
-  <si>
-    <t>leo</t>
-  </si>
-  <si>
-    <t>yan</t>
-  </si>
-  <si>
-    <t>leva</t>
-  </si>
-  <si>
-    <t>yun</t>
-  </si>
-  <si>
-    <t>ro</t>
-  </si>
-  <si>
-    <t>yon</t>
-  </si>
-  <si>
-    <t>log</t>
+    <t>R</t>
+  </si>
+  <si>
+    <t>rin</t>
+  </si>
+  <si>
+    <t>Ly</t>
+  </si>
+  <si>
+    <t>nte</t>
+  </si>
+  <si>
+    <t>Od</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>Le</t>
+  </si>
+  <si>
+    <t>aus</t>
+  </si>
+  <si>
+    <t>Ezr</t>
+  </si>
+  <si>
+    <t>ara</t>
+  </si>
+  <si>
+    <t>Ir</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>ye</t>
+  </si>
+  <si>
+    <t>Ju</t>
+  </si>
+  <si>
+    <t>ien</t>
+  </si>
+  <si>
+    <t>Th</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>Ei</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>Da</t>
+  </si>
+  <si>
+    <t>ona</t>
+  </si>
+  <si>
+    <t>Fr</t>
+  </si>
+  <si>
+    <t>ura</t>
+  </si>
+  <si>
+    <t>Nar</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>Ez</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>Ay</t>
+  </si>
+  <si>
+    <t>ien</t>
+  </si>
+  <si>
+    <t>Ta</t>
   </si>
   <si>
     <t>ra</t>
   </si>
   <si>
-    <t>rossi</t>
-  </si>
-  <si>
-    <t>larg</t>
-  </si>
-  <si>
-    <t>lova</t>
-  </si>
-  <si>
-    <t>lard</t>
-  </si>
-  <si>
-    <t>robe</t>
-  </si>
-  <si>
-    <t>rice</t>
-  </si>
-  <si>
-    <t>wa</t>
-  </si>
-  <si>
-    <t>ly</t>
-  </si>
-  <si>
-    <t>wag</t>
-  </si>
-  <si>
-    <t>lag</t>
-  </si>
-  <si>
-    <t>wy</t>
-  </si>
-  <si>
-    <t>lass</t>
-  </si>
-  <si>
-    <t>ail</t>
-  </si>
-  <si>
-    <t>rak</t>
-  </si>
-  <si>
-    <t>eil</t>
-  </si>
-  <si>
-    <t>letta</t>
-  </si>
-  <si>
-    <t>eo</t>
-  </si>
-  <si>
-    <t>rana</t>
-  </si>
-  <si>
-    <t>io</t>
-  </si>
-  <si>
-    <t>raf</t>
-  </si>
-  <si>
-    <t>ol</t>
-  </si>
-  <si>
-    <t>ralk</t>
-  </si>
-  <si>
-    <t>zerg</t>
-  </si>
-  <si>
-    <t>rald</t>
-  </si>
-  <si>
-    <t>zi</t>
-  </si>
-  <si>
-    <t>li</t>
-  </si>
-  <si>
-    <t>wi</t>
-  </si>
-  <si>
-    <t>ria</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>line</t>
-  </si>
-  <si>
-    <t>win</t>
-  </si>
-  <si>
-    <t>lite</t>
-  </si>
-  <si>
-    <t>din</t>
-  </si>
-  <si>
-    <t>liss</t>
-  </si>
-  <si>
-    <t>deo</t>
-  </si>
-  <si>
-    <t>liz</t>
-  </si>
-  <si>
-    <t>dao</t>
-  </si>
-  <si>
-    <t>rick</t>
-  </si>
-  <si>
-    <t>seth</t>
-  </si>
-  <si>
-    <t>ritta</t>
-  </si>
-  <si>
-    <t>ago</t>
-  </si>
-  <si>
-    <t>rul</t>
-  </si>
-  <si>
-    <t>aga</t>
-  </si>
-  <si>
-    <t>lur</t>
-  </si>
-  <si>
-    <t>nes</t>
-  </si>
-  <si>
-    <t>ruin</t>
-  </si>
-  <si>
-    <t>nis</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>mis</t>
-  </si>
-  <si>
-    <t>loss</t>
-  </si>
-  <si>
-    <t>mah</t>
-  </si>
-  <si>
-    <t>loot</t>
-  </si>
-  <si>
-    <t>lah</t>
-  </si>
-  <si>
-    <t>ry</t>
-  </si>
-  <si>
-    <t>teo</t>
-  </si>
-  <si>
-    <t>rea</t>
-  </si>
-  <si>
-    <t>meo</t>
-  </si>
-  <si>
-    <t>rey</t>
+    <t>Br</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>Pho</t>
+  </si>
+  <si>
+    <t>ron</t>
+  </si>
+  <si>
+    <t>Br</t>
+  </si>
+  <si>
+    <t>ara</t>
+  </si>
+  <si>
+    <t>Sel</t>
+  </si>
+  <si>
+    <t>yla</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>ri</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>wan</t>
+  </si>
+  <si>
+    <t>Lo</t>
+  </si>
+  <si>
+    <t>ia</t>
+  </si>
+  <si>
+    <t>El</t>
+  </si>
+  <si>
+    <t>sia</t>
+  </si>
+  <si>
+    <t>Am</t>
+  </si>
+  <si>
+    <t>vi</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>vi</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t>el</t>
   </si>
   <si>
-    <t>ler</t>
-  </si>
-  <si>
-    <t>es</t>
-  </si>
-  <si>
-    <t>ress</t>
-  </si>
-  <si>
-    <t>ken</t>
-  </si>
-  <si>
-    <t>lez</t>
-  </si>
-  <si>
-    <t>van</t>
-  </si>
-  <si>
-    <t>retta</t>
-  </si>
-  <si>
-    <t>ves</t>
-  </si>
-  <si>
-    <t>rel</t>
-  </si>
-  <si>
-    <t>vas</t>
-  </si>
-  <si>
-    <t>law</t>
-  </si>
-  <si>
-    <t>vos</t>
-  </si>
-  <si>
-    <t>loa</t>
-  </si>
-  <si>
-    <t>bos</t>
-  </si>
-  <si>
-    <t>roy</t>
-  </si>
-  <si>
-    <t>los</t>
-  </si>
-  <si>
-    <t>roer</t>
-  </si>
-  <si>
-    <t>ros</t>
-  </si>
-  <si>
-    <t>lerg</t>
-  </si>
-  <si>
-    <t>jos</t>
-  </si>
-  <si>
-    <t>lort</t>
-  </si>
-  <si>
-    <t>jes</t>
-  </si>
-  <si>
-    <t>rot</t>
-  </si>
-  <si>
-    <t>beth</t>
-  </si>
-  <si>
-    <t>lord</t>
-  </si>
-  <si>
-    <t>old</t>
-  </si>
-  <si>
-    <t>log</t>
-  </si>
-  <si>
-    <t>ald</t>
-  </si>
-  <si>
-    <t>loth</t>
-  </si>
-  <si>
-    <t>kol</t>
-  </si>
-  <si>
-    <t>loz</t>
-  </si>
-  <si>
-    <t>cy</t>
-  </si>
-  <si>
-    <t>rock</t>
-  </si>
-  <si>
-    <t>ce</t>
-  </si>
-  <si>
-    <t>rotta</t>
-  </si>
-  <si>
-    <t>se</t>
-  </si>
-  <si>
-    <t>lot</t>
-  </si>
-  <si>
-    <t>hog</t>
-  </si>
-  <si>
-    <t>rona</t>
-  </si>
-  <si>
-    <t>mos</t>
-  </si>
-  <si>
-    <t>rof</t>
-  </si>
-  <si>
-    <t>wes</t>
-  </si>
-  <si>
-    <t>ron</t>
-  </si>
-  <si>
-    <t>po</t>
-  </si>
-  <si>
-    <t>lond</t>
-  </si>
-  <si>
-    <t>pi</t>
-  </si>
-  <si>
-    <t>wer</t>
-  </si>
-  <si>
-    <t>fis</t>
-  </si>
-  <si>
-    <t>wert</t>
-  </si>
-  <si>
-    <t>wis</t>
-  </si>
-  <si>
-    <t>wart</t>
-  </si>
-  <si>
-    <t>ray</t>
-  </si>
-  <si>
-    <t>ward</t>
-  </si>
-  <si>
-    <t>lay</t>
-  </si>
-  <si>
-    <t>won</t>
-  </si>
-  <si>
-    <t>les</t>
-  </si>
-  <si>
-    <t>er</t>
-  </si>
-  <si>
-    <t>ro</t>
-  </si>
-  <si>
-    <t>chael</t>
-  </si>
-  <si>
-    <t>stan</t>
-  </si>
-  <si>
-    <t>tony</t>
-  </si>
-  <si>
-    <t>dun</t>
-  </si>
-  <si>
-    <t>nsor</t>
-  </si>
-  <si>
-    <t>gun</t>
-  </si>
-  <si>
-    <t>seth</t>
-  </si>
-  <si>
-    <t>kay</t>
-  </si>
-  <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>bay</t>
-  </si>
-  <si>
-    <t>ba</t>
+    <t>Ra</t>
+  </si>
+  <si>
+    <t>yx</t>
+  </si>
+  <si>
+    <t>Ga</t>
+  </si>
+  <si>
+    <t>eve</t>
   </si>
 </sst>
 </file>
@@ -1649,10 +1655,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1933,10 +1942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B266"/>
+  <dimension ref="A1:F267"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1944,23 +1953,23 @@
     <col min="1" max="16384" width="14.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1968,7 +1977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1976,7 +1985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1984,7 +1993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1992,15 +2001,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -2008,7 +2018,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -2016,7 +2026,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -2024,7 +2034,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -2032,7 +2042,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
@@ -2040,7 +2050,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -2048,7 +2058,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -2056,7 +2066,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -2216,7 +2226,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="12.75">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>66</v>
       </c>
@@ -4062,6 +4072,14 @@
       </c>
       <c r="B266" s="1" t="s">
         <v>527</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="12.75">
+      <c r="A267" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>